<commit_message>
Assignment 2 + Assignment 1 with graphs
</commit_message>
<xml_diff>
--- a/PROJECT/Entrega/input16_Ex2.xlsx
+++ b/PROJECT/Entrega/input16_Ex2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Javier Aguilar\OneDrive - UPV\AE4423 Airline Planning\Project\Codes\Exercise2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo\Desktop\TU DELFT asignaturas\Q2\AE4423-19 Airline Planning and Optimization\Assignment 1\AirlinePlanningAssignment\PROJECT\Entrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E2B5931-1BA5-430A-B562-6C42A562AC7F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5405086B-363E-4623-8828-264ADD2727E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="4" xr2:uid="{17AC5D55-CFD6-48D2-82F3-9F35A47B361D}"/>
+    <workbookView xWindow="2484" yWindow="2004" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="3" xr2:uid="{17AC5D55-CFD6-48D2-82F3-9F35A47B361D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="2" r:id="rId1"/>
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -729,9 +729,9 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -753,7 +753,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>71</v>
       </c>
@@ -774,7 +774,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -795,7 +795,7 @@
         <v>39720.44342678359</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -816,7 +816,7 @@
         <v>38476.658636157503</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -837,7 +837,7 @@
         <v>48223.155494182516</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -858,7 +858,7 @@
         <v>44469.909060724385</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -879,7 +879,7 @@
         <v>28156.815836235186</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -900,7 +900,7 @@
         <v>28156.815836235186</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -921,7 +921,7 @@
         <v>44469.909060724385</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -942,7 +942,7 @@
         <v>31952.975920684112</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -963,7 +963,7 @@
         <v>69330.690154491196</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -984,7 +984,7 @@
         <v>53442.008280802183</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>21136.297210200468</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>44469.909060724385</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>45703.32786507401</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>13811.664243680832</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>39720.44342678359</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>10813.716600198628</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>18613.423873381744</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>70056.873391621339</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>31952.975920684101</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>21136.297210200468</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>59531.661964344021</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>59531.661964344021</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>59531.661964344021</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1291,9 +1291,9 @@
       <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1392,7 +1392,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>30</v>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>55</v>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>56</v>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>57</v>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>58</v>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1895,7 +1895,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>59</v>
@@ -1934,7 +1934,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>2</v>
@@ -1973,7 +1973,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>31</v>
@@ -2105,7 +2105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>32</v>
@@ -2171,7 +2171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>33</v>
@@ -2237,7 +2237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>34</v>
@@ -2303,7 +2303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>35</v>
@@ -2369,7 +2369,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>36</v>
@@ -2435,7 +2435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>37</v>
@@ -2501,7 +2501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>38</v>
@@ -2567,7 +2567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>39</v>
@@ -2633,7 +2633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>40</v>
@@ -2699,7 +2699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>41</v>
@@ -2765,7 +2765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>42</v>
@@ -2831,7 +2831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>43</v>
@@ -2897,7 +2897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>44</v>
@@ -2963,7 +2963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>45</v>
@@ -3029,7 +3029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>46</v>
@@ -3095,7 +3095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>47</v>
@@ -3161,7 +3161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>48</v>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>49</v>
@@ -3293,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>50</v>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>32</v>
@@ -3595,7 +3595,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>33</v>
@@ -3673,7 +3673,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>34</v>
@@ -3751,7 +3751,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>35</v>
@@ -3829,7 +3829,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>36</v>
@@ -3907,7 +3907,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>37</v>
@@ -3985,7 +3985,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>38</v>
@@ -4063,7 +4063,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>39</v>
@@ -4141,7 +4141,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>40</v>
@@ -4219,7 +4219,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
         <v>41</v>
@@ -4297,7 +4297,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>42</v>
@@ -4375,7 +4375,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>43</v>
@@ -4453,7 +4453,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>44</v>
@@ -4531,7 +4531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>45</v>
@@ -4609,7 +4609,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
         <v>46</v>
@@ -4687,7 +4687,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
         <v>47</v>
@@ -4765,7 +4765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>48</v>
@@ -4843,7 +4843,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>49</v>
@@ -4921,7 +4921,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
         <v>50</v>
@@ -4999,7 +4999,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>51</v>
@@ -5077,7 +5077,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
         <v>52</v>
@@ -5155,7 +5155,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
         <v>53</v>
@@ -5233,7 +5233,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
         <v>54</v>
@@ -5311,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -5339,7 +5339,7 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
         <v>32</v>
@@ -5575,7 +5575,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>33</v>
@@ -5653,7 +5653,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
         <v>34</v>
@@ -5731,7 +5731,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
         <v>35</v>
@@ -5809,7 +5809,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
         <v>36</v>
@@ -5887,7 +5887,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
         <v>37</v>
@@ -5965,7 +5965,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
         <v>38</v>
@@ -6043,7 +6043,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
         <v>39</v>
@@ -6121,7 +6121,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
         <v>40</v>
@@ -6199,7 +6199,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
         <v>41</v>
@@ -6277,7 +6277,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
         <v>42</v>
@@ -6355,7 +6355,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
         <v>43</v>
@@ -6433,7 +6433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
         <v>44</v>
@@ -6511,7 +6511,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
         <v>45</v>
@@ -6589,7 +6589,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
         <v>46</v>
@@ -6667,7 +6667,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
         <v>47</v>
@@ -6745,7 +6745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
         <v>48</v>
@@ -6823,7 +6823,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
         <v>49</v>
@@ -6901,7 +6901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
         <v>50</v>
@@ -6979,7 +6979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
         <v>51</v>
@@ -7057,7 +7057,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
         <v>52</v>
@@ -7135,7 +7135,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
         <v>53</v>
@@ -7213,7 +7213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
         <v>54</v>
@@ -7291,7 +7291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -7319,7 +7319,7 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>68</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1" t="s">
         <v>31</v>
@@ -7475,7 +7475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1" t="s">
         <v>32</v>
@@ -7553,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1" t="s">
         <v>33</v>
@@ -7631,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1" t="s">
         <v>34</v>
@@ -7709,7 +7709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
         <v>35</v>
@@ -7787,7 +7787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1" t="s">
         <v>36</v>
@@ -7865,7 +7865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="B95" s="1" t="s">
         <v>37</v>
@@ -7943,7 +7943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="B96" s="1" t="s">
         <v>38</v>
@@ -8021,7 +8021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
       <c r="B97" s="1" t="s">
         <v>39</v>
@@ -8099,7 +8099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
       <c r="B98" s="1" t="s">
         <v>40</v>
@@ -8177,7 +8177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
       <c r="B99" s="1" t="s">
         <v>41</v>
@@ -8255,7 +8255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
         <v>42</v>
@@ -8333,7 +8333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
         <v>43</v>
@@ -8411,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
       <c r="B102" s="1" t="s">
         <v>44</v>
@@ -8489,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A103" s="1"/>
       <c r="B103" s="1" t="s">
         <v>45</v>
@@ -8567,7 +8567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A104" s="1"/>
       <c r="B104" s="1" t="s">
         <v>46</v>
@@ -8645,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A105" s="1"/>
       <c r="B105" s="1" t="s">
         <v>47</v>
@@ -8723,7 +8723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A106" s="1"/>
       <c r="B106" s="1" t="s">
         <v>48</v>
@@ -8801,7 +8801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A107" s="1"/>
       <c r="B107" s="1" t="s">
         <v>49</v>
@@ -8879,7 +8879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A108" s="1"/>
       <c r="B108" s="1" t="s">
         <v>50</v>
@@ -8957,7 +8957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A109" s="1"/>
       <c r="B109" s="1" t="s">
         <v>51</v>
@@ -9035,7 +9035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A110" s="1"/>
       <c r="B110" s="1" t="s">
         <v>52</v>
@@ -9113,7 +9113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A111" s="1"/>
       <c r="B111" s="1" t="s">
         <v>53</v>
@@ -9191,7 +9191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A112" s="1"/>
       <c r="B112" s="1" t="s">
         <v>54</v>
@@ -9282,12 +9282,12 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>88</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -9327,7 +9327,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -9347,7 +9347,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -9367,7 +9367,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -9407,7 +9407,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>290000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -9496,13 +9496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DCFAE1-DFC4-492D-9E85-3B861F1E6777}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -9660,7 +9660,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -9738,7 +9738,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>33</v>
@@ -9816,7 +9816,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>34</v>
@@ -9894,7 +9894,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -9972,7 +9972,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
@@ -10050,7 +10050,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>37</v>
@@ -10128,7 +10128,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>38</v>
@@ -10206,7 +10206,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>39</v>
@@ -10284,7 +10284,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>40</v>
@@ -10362,7 +10362,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
@@ -10440,7 +10440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>42</v>
@@ -10518,7 +10518,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>43</v>
@@ -10596,7 +10596,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>44</v>
@@ -10674,7 +10674,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>45</v>
@@ -10752,7 +10752,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>46</v>
@@ -10830,7 +10830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>47</v>
@@ -10908,7 +10908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -10986,7 +10986,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>49</v>
@@ -11064,7 +11064,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>50</v>
@@ -11142,7 +11142,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>51</v>
@@ -11220,7 +11220,7 @@
         <v>4420</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>52</v>
@@ -11298,7 +11298,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>53</v>
@@ -11376,7 +11376,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>54</v>
@@ -11463,13 +11463,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD27000-8541-4781-89D6-9B7985E2D77B}">
   <dimension ref="A1:Y181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B158" sqref="B158:Y181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -11623,7 +11623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -11700,7 +11700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -11854,7 +11854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -11931,7 +11931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -12085,7 +12085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -12162,7 +12162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -12316,7 +12316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -12393,7 +12393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -12470,7 +12470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -12547,7 +12547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -12701,7 +12701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -12778,7 +12778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -12855,7 +12855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -12932,7 +12932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -13009,7 +13009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -13086,7 +13086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -13317,7 +13317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
@@ -13394,7 +13394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -13471,7 +13471,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -13625,7 +13625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -13856,7 +13856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -14010,7 +14010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -14087,7 +14087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -14164,7 +14164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -14241,7 +14241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -14318,7 +14318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -14395,7 +14395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -14472,7 +14472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -14549,7 +14549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -14626,7 +14626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -14780,7 +14780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -14857,7 +14857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -15011,7 +15011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -15165,7 +15165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -15242,7 +15242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -15319,7 +15319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>105</v>
       </c>
@@ -15396,7 +15396,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -15473,7 +15473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -15627,7 +15627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -15704,7 +15704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>35</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -15858,7 +15858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -15935,7 +15935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -16012,7 +16012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -16089,7 +16089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>40</v>
       </c>
@@ -16166,7 +16166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -16243,7 +16243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -16397,7 +16397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>44</v>
       </c>
@@ -16474,7 +16474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>45</v>
       </c>
@@ -16551,7 +16551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>46</v>
       </c>
@@ -16628,7 +16628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>47</v>
       </c>
@@ -16705,7 +16705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -16782,7 +16782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>49</v>
       </c>
@@ -16859,7 +16859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>50</v>
       </c>
@@ -16936,7 +16936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>51</v>
       </c>
@@ -17013,7 +17013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>52</v>
       </c>
@@ -17090,7 +17090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>53</v>
       </c>
@@ -17167,7 +17167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>54</v>
       </c>
@@ -17244,7 +17244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -17321,7 +17321,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -17398,7 +17398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>32</v>
       </c>
@@ -17475,7 +17475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -17552,7 +17552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -17629,7 +17629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>35</v>
       </c>
@@ -17706,7 +17706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>36</v>
       </c>
@@ -17783,7 +17783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -17860,7 +17860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>38</v>
       </c>
@@ -17937,7 +17937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -18014,7 +18014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>40</v>
       </c>
@@ -18091,7 +18091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -18168,7 +18168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -18245,7 +18245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>43</v>
       </c>
@@ -18322,7 +18322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>44</v>
       </c>
@@ -18399,7 +18399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -18476,7 +18476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>46</v>
       </c>
@@ -18553,7 +18553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -18707,7 +18707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>49</v>
       </c>
@@ -18784,7 +18784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>50</v>
       </c>
@@ -18861,7 +18861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>51</v>
       </c>
@@ -18938,7 +18938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>52</v>
       </c>
@@ -19015,7 +19015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>53</v>
       </c>
@@ -19092,7 +19092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>54</v>
       </c>
@@ -19169,7 +19169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -19246,7 +19246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>31</v>
       </c>
@@ -19323,7 +19323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>32</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>33</v>
       </c>
@@ -19477,7 +19477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>34</v>
       </c>
@@ -19554,7 +19554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>35</v>
       </c>
@@ -19631,7 +19631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>36</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>37</v>
       </c>
@@ -19785,7 +19785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>38</v>
       </c>
@@ -19862,7 +19862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -19939,7 +19939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>40</v>
       </c>
@@ -20016,7 +20016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>41</v>
       </c>
@@ -20093,7 +20093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>42</v>
       </c>
@@ -20170,7 +20170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>43</v>
       </c>
@@ -20247,7 +20247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>44</v>
       </c>
@@ -20324,7 +20324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>45</v>
       </c>
@@ -20401,7 +20401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>46</v>
       </c>
@@ -20478,7 +20478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>47</v>
       </c>
@@ -20555,7 +20555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -20632,7 +20632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>49</v>
       </c>
@@ -20709,7 +20709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>50</v>
       </c>
@@ -20786,7 +20786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>51</v>
       </c>
@@ -20863,7 +20863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>52</v>
       </c>
@@ -20940,7 +20940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>53</v>
       </c>
@@ -21017,7 +21017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>54</v>
       </c>
@@ -21094,7 +21094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>108</v>
       </c>
@@ -21171,7 +21171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>31</v>
       </c>
@@ -21248,7 +21248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>32</v>
       </c>
@@ -21325,7 +21325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -21402,7 +21402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>34</v>
       </c>
@@ -21479,7 +21479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>35</v>
       </c>
@@ -21556,7 +21556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>36</v>
       </c>
@@ -21633,7 +21633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>37</v>
       </c>
@@ -21710,7 +21710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>38</v>
       </c>
@@ -21787,7 +21787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>39</v>
       </c>
@@ -21864,7 +21864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>40</v>
       </c>
@@ -21941,7 +21941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>41</v>
       </c>
@@ -22018,7 +22018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>42</v>
       </c>
@@ -22095,7 +22095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>43</v>
       </c>
@@ -22172,7 +22172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>44</v>
       </c>
@@ -22249,7 +22249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>45</v>
       </c>
@@ -22326,7 +22326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>46</v>
       </c>
@@ -22403,7 +22403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>47</v>
       </c>
@@ -22480,7 +22480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>48</v>
       </c>
@@ -22557,7 +22557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>49</v>
       </c>
@@ -22634,7 +22634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>50</v>
       </c>
@@ -22711,7 +22711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>51</v>
       </c>
@@ -22788,7 +22788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>52</v>
       </c>
@@ -22865,7 +22865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>53</v>
       </c>
@@ -22942,7 +22942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>54</v>
       </c>
@@ -23019,7 +23019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>107</v>
       </c>
@@ -23096,7 +23096,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>31</v>
       </c>
@@ -23173,7 +23173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>32</v>
       </c>
@@ -23250,7 +23250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>33</v>
       </c>
@@ -23327,7 +23327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>34</v>
       </c>
@@ -23404,7 +23404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>35</v>
       </c>
@@ -23481,7 +23481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>36</v>
       </c>
@@ -23558,7 +23558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>37</v>
       </c>
@@ -23635,7 +23635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>38</v>
       </c>
@@ -23712,7 +23712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>39</v>
       </c>
@@ -23789,7 +23789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>40</v>
       </c>
@@ -23866,7 +23866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>41</v>
       </c>
@@ -23943,7 +23943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>42</v>
       </c>
@@ -24020,7 +24020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>43</v>
       </c>
@@ -24097,7 +24097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>44</v>
       </c>
@@ -24174,7 +24174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>45</v>
       </c>
@@ -24251,7 +24251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>46</v>
       </c>
@@ -24328,7 +24328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>47</v>
       </c>
@@ -24405,7 +24405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -24482,7 +24482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>49</v>
       </c>
@@ -24559,7 +24559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>50</v>
       </c>
@@ -24636,7 +24636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>51</v>
       </c>
@@ -24713,7 +24713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>52</v>
       </c>
@@ -24790,7 +24790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>53</v>
       </c>
@@ -24867,7 +24867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>54</v>
       </c>

</xml_diff>